<commit_message>
update template, change autofill for new columns, add confirm, checkboxes
</commit_message>
<xml_diff>
--- a/src/com/aquino/webParser/resources/template/TEMPLATE_FOR_JWP.xlsx
+++ b/src/com/aquino/webParser/resources/template/TEMPLATE_FOR_JWP.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\book\clone\src\com\aquino\webParser\resources\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64E89B0-4BE0-49C8-A9FA-838262C4695F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6675" yWindow="4215" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,318 +12,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-    <author>User</author>
-  </authors>
-  <commentList>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Language book is written in
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>What is the language the book originally written as, eg, German</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-MM/DD/Y</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">MSRP
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-List price on BW</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>URL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Preschool
-5-8
-9-10
-Youth
-Adult
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">width x length x height
-in CM </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Paperback
-Hardcover
-Spiral Bound
-Continuous Fold
-Board Book
-see choices in /admin</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AI1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Input "number" only OR "p" next to the number</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">mm/dd/yy
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AK1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-See BW Awards code</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">in Pounds
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">see /admin for choices
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AN1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-See admin code </t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,9 +139,6 @@
     <t>Author 2 (BW)</t>
   </si>
   <si>
-    <t>Publisher Id</t>
-  </si>
-  <si>
     <t>Publisher (Store)</t>
   </si>
   <si>
@@ -469,15 +150,18 @@
   <si>
     <t>Author 2</t>
   </si>
+  <si>
+    <t>Publisher</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,32 +173,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -592,7 +250,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -602,13 +260,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -617,10 +275,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -629,7 +287,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -638,7 +296,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -646,9 +304,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
-    <cellStyle name="一般_Sheet1_2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般_Sheet1_2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -683,7 +341,7 @@
         <xdr:cNvPr id="2" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -735,7 +393,7 @@
         <xdr:cNvPr id="3" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -787,7 +445,7 @@
         <xdr:cNvPr id="4" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -839,7 +497,7 @@
         <xdr:cNvPr id="5" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -891,7 +549,7 @@
         <xdr:cNvPr id="6" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -943,7 +601,7 @@
         <xdr:cNvPr id="7" name="Picture 180" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -995,7 +653,7 @@
         <xdr:cNvPr id="8" name="Picture 181" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1047,7 +705,7 @@
         <xdr:cNvPr id="9" name="Picture 182" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1099,7 +757,7 @@
         <xdr:cNvPr id="10" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1151,7 +809,7 @@
         <xdr:cNvPr id="11" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1203,7 +861,7 @@
         <xdr:cNvPr id="12" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,7 +913,7 @@
         <xdr:cNvPr id="13" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1307,7 +965,7 @@
         <xdr:cNvPr id="14" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1017,7 @@
         <xdr:cNvPr id="15" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1411,7 +1069,7 @@
         <xdr:cNvPr id="16" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1463,7 +1121,7 @@
         <xdr:cNvPr id="17" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1515,7 +1173,7 @@
         <xdr:cNvPr id="18" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1567,7 +1225,7 @@
         <xdr:cNvPr id="19" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1619,7 +1277,7 @@
         <xdr:cNvPr id="20" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,7 +1329,7 @@
         <xdr:cNvPr id="21" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1723,7 +1381,7 @@
         <xdr:cNvPr id="22" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1775,7 +1433,7 @@
         <xdr:cNvPr id="23" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1827,7 +1485,7 @@
         <xdr:cNvPr id="24" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1879,7 +1537,7 @@
         <xdr:cNvPr id="25" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1931,7 +1589,7 @@
         <xdr:cNvPr id="26" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1983,7 +1641,7 @@
         <xdr:cNvPr id="27" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2035,7 +1693,7 @@
         <xdr:cNvPr id="28" name="Picture 201" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2087,7 +1745,7 @@
         <xdr:cNvPr id="29" name="Picture 202" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2139,7 +1797,7 @@
         <xdr:cNvPr id="30" name="Picture 203" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2191,7 +1849,7 @@
         <xdr:cNvPr id="31" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2243,7 +1901,7 @@
         <xdr:cNvPr id="32" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2295,7 +1953,7 @@
         <xdr:cNvPr id="33" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2347,7 +2005,7 @@
         <xdr:cNvPr id="34" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2399,7 +2057,7 @@
         <xdr:cNvPr id="35" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2451,7 +2109,7 @@
         <xdr:cNvPr id="36" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2503,7 +2161,7 @@
         <xdr:cNvPr id="37" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2555,7 +2213,7 @@
         <xdr:cNvPr id="38" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2607,7 +2265,7 @@
         <xdr:cNvPr id="39" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2659,7 +2317,7 @@
         <xdr:cNvPr id="40" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2711,7 +2369,7 @@
         <xdr:cNvPr id="41" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2763,7 +2421,7 @@
         <xdr:cNvPr id="42" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2815,7 +2473,7 @@
         <xdr:cNvPr id="43" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2867,7 +2525,7 @@
         <xdr:cNvPr id="44" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2919,7 +2577,7 @@
         <xdr:cNvPr id="45" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2971,7 +2629,7 @@
         <xdr:cNvPr id="46" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3023,7 +2681,7 @@
         <xdr:cNvPr id="47" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3075,7 +2733,7 @@
         <xdr:cNvPr id="48" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3127,7 +2785,7 @@
         <xdr:cNvPr id="49" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3179,7 +2837,7 @@
         <xdr:cNvPr id="50" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000032000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3231,7 +2889,7 @@
         <xdr:cNvPr id="51" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000033000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3283,7 +2941,7 @@
         <xdr:cNvPr id="52" name="Picture 225" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3335,7 +2993,7 @@
         <xdr:cNvPr id="53" name="Picture 226" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3387,7 +3045,7 @@
         <xdr:cNvPr id="54" name="Picture 227" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000036000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3439,7 +3097,7 @@
         <xdr:cNvPr id="55" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3491,7 +3149,7 @@
         <xdr:cNvPr id="56" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3543,7 +3201,7 @@
         <xdr:cNvPr id="57" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000039000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3595,7 +3253,7 @@
         <xdr:cNvPr id="58" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3647,7 +3305,7 @@
         <xdr:cNvPr id="59" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3699,7 +3357,7 @@
         <xdr:cNvPr id="60" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3751,7 +3409,7 @@
         <xdr:cNvPr id="61" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3803,7 +3461,7 @@
         <xdr:cNvPr id="62" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3855,7 +3513,7 @@
         <xdr:cNvPr id="63" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3907,7 +3565,7 @@
         <xdr:cNvPr id="64" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000040000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3959,7 +3617,7 @@
         <xdr:cNvPr id="65" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000041000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4011,7 +3669,7 @@
         <xdr:cNvPr id="66" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4063,7 +3721,7 @@
         <xdr:cNvPr id="67" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000043000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4115,7 +3773,7 @@
         <xdr:cNvPr id="68" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000044000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4167,7 +3825,7 @@
         <xdr:cNvPr id="69" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4219,7 +3877,7 @@
         <xdr:cNvPr id="70" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000046000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4271,7 +3929,7 @@
         <xdr:cNvPr id="71" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4323,7 +3981,7 @@
         <xdr:cNvPr id="72" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000048000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4375,7 +4033,7 @@
         <xdr:cNvPr id="73" name="Picture 246" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000049000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4427,7 +4085,7 @@
         <xdr:cNvPr id="74" name="Picture 247" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4479,7 +4137,7 @@
         <xdr:cNvPr id="75" name="Picture 248" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4531,7 +4189,7 @@
         <xdr:cNvPr id="76" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4583,7 +4241,7 @@
         <xdr:cNvPr id="77" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4635,7 +4293,7 @@
         <xdr:cNvPr id="78" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4687,7 +4345,7 @@
         <xdr:cNvPr id="79" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4739,7 +4397,7 @@
         <xdr:cNvPr id="80" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000050000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4791,7 +4449,7 @@
         <xdr:cNvPr id="81" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000051000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4843,7 +4501,7 @@
         <xdr:cNvPr id="82" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4895,7 +4553,7 @@
         <xdr:cNvPr id="83" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4947,7 +4605,7 @@
         <xdr:cNvPr id="84" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000054000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4999,7 +4657,7 @@
         <xdr:cNvPr id="85" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5051,7 +4709,7 @@
         <xdr:cNvPr id="86" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000056000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5103,7 +4761,7 @@
         <xdr:cNvPr id="87" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000057000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5155,7 +4813,7 @@
         <xdr:cNvPr id="88" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000058000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5207,7 +4865,7 @@
         <xdr:cNvPr id="89" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000059000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000059000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5259,7 +4917,7 @@
         <xdr:cNvPr id="90" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5311,7 +4969,7 @@
         <xdr:cNvPr id="91" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5363,7 +5021,7 @@
         <xdr:cNvPr id="92" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5415,7 +5073,7 @@
         <xdr:cNvPr id="93" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5467,7 +5125,7 @@
         <xdr:cNvPr id="94" name="Picture 267" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5519,7 +5177,7 @@
         <xdr:cNvPr id="95" name="Picture 268" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5571,7 +5229,7 @@
         <xdr:cNvPr id="96" name="Picture 269" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000060000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5623,7 +5281,7 @@
         <xdr:cNvPr id="97" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5675,7 +5333,7 @@
         <xdr:cNvPr id="98" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000062000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5727,7 +5385,7 @@
         <xdr:cNvPr id="99" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000063000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5779,7 +5437,7 @@
         <xdr:cNvPr id="100" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000064000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000064000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5831,7 +5489,7 @@
         <xdr:cNvPr id="101" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000065000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5883,7 +5541,7 @@
         <xdr:cNvPr id="102" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000066000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000066000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5935,7 +5593,7 @@
         <xdr:cNvPr id="103" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000067000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5987,7 +5645,7 @@
         <xdr:cNvPr id="104" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000068000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000068000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6039,7 +5697,7 @@
         <xdr:cNvPr id="105" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6091,7 +5749,7 @@
         <xdr:cNvPr id="106" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6143,7 +5801,7 @@
         <xdr:cNvPr id="107" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6195,7 +5853,7 @@
         <xdr:cNvPr id="108" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6247,7 +5905,7 @@
         <xdr:cNvPr id="109" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6299,7 +5957,7 @@
         <xdr:cNvPr id="110" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6351,7 +6009,7 @@
         <xdr:cNvPr id="111" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6403,7 +6061,7 @@
         <xdr:cNvPr id="112" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000070000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000070000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6455,7 +6113,7 @@
         <xdr:cNvPr id="113" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000071000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6507,7 +6165,7 @@
         <xdr:cNvPr id="114" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000072000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6559,7 +6217,7 @@
         <xdr:cNvPr id="115" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6611,7 +6269,7 @@
         <xdr:cNvPr id="116" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000074000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000074000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6663,7 +6321,7 @@
         <xdr:cNvPr id="117" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000075000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6715,7 +6373,7 @@
         <xdr:cNvPr id="118" name="Picture 291" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000076000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000076000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6767,7 +6425,7 @@
         <xdr:cNvPr id="119" name="Picture 292" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000077000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000077000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6819,7 +6477,7 @@
         <xdr:cNvPr id="120" name="Picture 293" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000078000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000078000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6871,7 +6529,7 @@
         <xdr:cNvPr id="121" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000079000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000079000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6923,7 +6581,7 @@
         <xdr:cNvPr id="122" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6975,7 +6633,7 @@
         <xdr:cNvPr id="123" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7027,7 +6685,7 @@
         <xdr:cNvPr id="124" name="Picture 6" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7079,7 +6737,7 @@
         <xdr:cNvPr id="125" name="Picture 7" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7131,7 +6789,7 @@
         <xdr:cNvPr id="126" name="Picture 8" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7183,7 +6841,7 @@
         <xdr:cNvPr id="127" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7235,7 +6893,7 @@
         <xdr:cNvPr id="128" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000080000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7287,7 +6945,7 @@
         <xdr:cNvPr id="129" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000081000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7339,7 +6997,7 @@
         <xdr:cNvPr id="130" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000082000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7391,7 +7049,7 @@
         <xdr:cNvPr id="131" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000083000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7443,7 +7101,7 @@
         <xdr:cNvPr id="132" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000084000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7495,7 +7153,7 @@
         <xdr:cNvPr id="133" name="Picture 9" descr="Your browser may not support display of this image." hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000085000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000085000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7547,7 +7205,7 @@
         <xdr:cNvPr id="134" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000086000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000086000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7599,7 +7257,7 @@
         <xdr:cNvPr id="135" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000087000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000087000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7651,7 +7309,7 @@
         <xdr:cNvPr id="136" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000088000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000088000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7703,7 +7361,7 @@
         <xdr:cNvPr id="137" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000089000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000089000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7755,7 +7413,7 @@
         <xdr:cNvPr id="138" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7807,7 +7465,7 @@
         <xdr:cNvPr id="139" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7859,7 +7517,7 @@
         <xdr:cNvPr id="140" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7911,7 +7569,7 @@
         <xdr:cNvPr id="141" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7963,7 +7621,7 @@
         <xdr:cNvPr id="142" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8015,7 +7673,7 @@
         <xdr:cNvPr id="143" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8067,7 +7725,7 @@
         <xdr:cNvPr id="144" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000090000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000090000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8119,7 +7777,7 @@
         <xdr:cNvPr id="145" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000091000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000091000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8171,7 +7829,7 @@
         <xdr:cNvPr id="146" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000092000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000092000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8223,7 +7881,7 @@
         <xdr:cNvPr id="147" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000093000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000093000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8275,7 +7933,7 @@
         <xdr:cNvPr id="148" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000094000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000094000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8327,7 +7985,7 @@
         <xdr:cNvPr id="149" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000095000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000095000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8379,7 +8037,7 @@
         <xdr:cNvPr id="150" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000096000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000096000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8431,7 +8089,7 @@
         <xdr:cNvPr id="151" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000097000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000097000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8483,7 +8141,7 @@
         <xdr:cNvPr id="152" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000098000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000098000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8535,7 +8193,7 @@
         <xdr:cNvPr id="153" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000099000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000099000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8587,7 +8245,7 @@
         <xdr:cNvPr id="154" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00009A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8639,7 +8297,7 @@
         <xdr:cNvPr id="155" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00009B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8691,7 +8349,7 @@
         <xdr:cNvPr id="156" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00009C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8743,7 +8401,7 @@
         <xdr:cNvPr id="157" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00009D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8795,7 +8453,7 @@
         <xdr:cNvPr id="158" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00009E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8847,7 +8505,7 @@
         <xdr:cNvPr id="159" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00009F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8899,7 +8557,7 @@
         <xdr:cNvPr id="160" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A0000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A0000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8951,7 +8609,7 @@
         <xdr:cNvPr id="161" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A1000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A1000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9003,7 +8661,7 @@
         <xdr:cNvPr id="162" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A2000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A2000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9055,7 +8713,7 @@
         <xdr:cNvPr id="163" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A3000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A3000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9107,7 +8765,7 @@
         <xdr:cNvPr id="164" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A4000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A4000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9159,7 +8817,7 @@
         <xdr:cNvPr id="165" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A5000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A5000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9211,7 +8869,7 @@
         <xdr:cNvPr id="166" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A6000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A6000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9263,7 +8921,7 @@
         <xdr:cNvPr id="167" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A7000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A7000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9315,7 +8973,7 @@
         <xdr:cNvPr id="168" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A8000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A8000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9367,7 +9025,7 @@
         <xdr:cNvPr id="169" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A9000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000A9000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9419,7 +9077,7 @@
         <xdr:cNvPr id="170" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000AA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9471,7 +9129,7 @@
         <xdr:cNvPr id="171" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AB000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000AB000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9523,7 +9181,7 @@
         <xdr:cNvPr id="172" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AC000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000AC000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9575,7 +9233,7 @@
         <xdr:cNvPr id="173" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AD000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000AD000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9627,7 +9285,7 @@
         <xdr:cNvPr id="174" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AE000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000AE000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9679,7 +9337,7 @@
         <xdr:cNvPr id="175" name="Picture 9" descr="Your browser may not support display of this image.">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AF000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000AF000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9717,7 +9375,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9759,7 +9417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9791,27 +9449,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9843,24 +9483,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10036,15 +9658,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AT20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="5" customWidth="1"/>
@@ -10081,7 +9703,7 @@
     <col min="40" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -10110,7 +9732,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>36</v>
@@ -10119,7 +9741,7 @@
         <v>37</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>38</v>
@@ -10128,13 +9750,13 @@
         <v>39</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>9</v>
@@ -10219,80 +9841,80 @@
       </c>
       <c r="AT1" s="2"/>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46">
       <c r="Z2" s="6"/>
       <c r="AC2" s="8"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46">
       <c r="Z3" s="6"/>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46">
       <c r="Z4" s="6"/>
       <c r="AC4" s="8"/>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46">
       <c r="Z5" s="6"/>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46">
       <c r="Z6" s="6"/>
       <c r="AC6" s="8"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46">
       <c r="Z7" s="6"/>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46">
       <c r="Z8" s="6"/>
       <c r="AC8" s="8"/>
       <c r="AE8" s="12"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46">
       <c r="Z9" s="6"/>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46">
       <c r="Z10" s="6"/>
       <c r="AC10" s="8"/>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46">
       <c r="Z11" s="6"/>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46">
       <c r="Z12" s="6"/>
       <c r="AC12" s="8"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46">
       <c r="Z13" s="6"/>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46">
       <c r="Z14" s="6"/>
       <c r="AC14" s="8"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46">
       <c r="Z15" s="6"/>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46">
       <c r="Z16" s="6"/>
       <c r="AC16" s="8"/>
     </row>
-    <row r="17" spans="26:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="26:29">
       <c r="Z17" s="6"/>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="26:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="26:29">
       <c r="Z18" s="6"/>
       <c r="AC18" s="8"/>
     </row>
-    <row r="19" spans="26:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="26:29">
       <c r="Z19" s="6"/>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="26:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="26:29">
       <c r="Z20" s="6"/>
       <c r="AC20" s="13"/>
     </row>
@@ -10300,29 +9922,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>